<commit_message>
remove exp list, 5 tabs in all xlsx templates
</commit_message>
<xml_diff>
--- a/startup/xlsx/grid.xlsx
+++ b/startup/xlsx/grid.xlsx
@@ -11,7 +11,9 @@
     <sheet name="grid1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="grid2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="grid3" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Version history" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="grid4" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="grid5" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Version history" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +27,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -51,6 +53,19 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Do NOT change the value of this cell</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Listing the experimenters is no longer necessary.  The experimenter list will be drawn from the proposal.</t>
         </r>
       </text>
     </comment>
@@ -145,7 +160,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -171,6 +186,19 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Do NOT change the value of this cell</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Listing the experimenters is no longer necessary.  The experimenter list will be drawn from the proposal.</t>
         </r>
       </text>
     </comment>
@@ -265,7 +293,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author>BR</author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -291,6 +319,285 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Do NOT change the value of this cell</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Listing the experimenters is no longer necessary.  The experimenter list will be drawn from the proposal.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>BR</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Do NOT change the value of this cell!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Do NOT change the value of this cell</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Listing the experimenters is no longer necessary.  The experimenter list will be drawn from the proposal.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Default values for the motor parameters are NOT used. Specify motor positions explicitly in the cells below
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>BR</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Do NOT change the value of this cell!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Do NOT change the value of this cell</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Listing the experimenters is no longer necessary.  The experimenter list will be drawn from the proposal.</t>
         </r>
       </text>
     </comment>
@@ -383,7 +690,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="79">
   <si>
     <t xml:space="preserve">Grid</t>
   </si>
@@ -541,7 +848,7 @@
     <t xml:space="preserve">unfocused</t>
   </si>
   <si>
-    <t xml:space="preserve">YBa2Cu3O7</t>
+    <t xml:space="preserve">X2O3</t>
   </si>
   <si>
     <t xml:space="preserve">powder on tape</t>
@@ -618,6 +925,9 @@
   <si>
     <t xml:space="preserve">add columns for sample X/Y + slit W/H to all spreadsheet types, also remove “Change edge at start?” + deprecate e0 column + deprecate single wheel spreadsheet</t>
   </si>
+  <si>
+    <t xml:space="preserve">remove experimenters cell, 5 tabs in template</t>
+  </si>
 </sst>
 </file>
 
@@ -628,7 +938,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -653,6 +963,14 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFDDDDDD"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -701,19 +1019,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF99FF"/>
-        <bgColor rgb="FFCC99FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFF66"/>
-        <bgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFE0C2CD"/>
       </patternFill>
     </fill>
     <fill>
@@ -725,13 +1037,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFDBB6"/>
-        <bgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFE0C2CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFF66"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -1012,19 +1330,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1048,23 +1366,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1116,83 +1434,83 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1240,7 +1558,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1248,7 +1566,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1294,7 +1612,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFE0C2CD"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1309,7 +1627,7 @@
       <rgbColor rgb="FFCCFF66"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99FF"/>
-      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFE0C2CD"/>
       <rgbColor rgb="FFFFDBB6"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
@@ -1343,9 +1661,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1082880</xdr:colOff>
+      <xdr:colOff>1081800</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>55800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1354,8 +1672,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3195360" y="7013160"/>
-          <a:ext cx="6929640" cy="1850400"/>
+          <a:off x="3198600" y="7013520"/>
+          <a:ext cx="6931800" cy="1848960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1377,7 +1695,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -1598,9 +1916,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1188000</xdr:colOff>
+      <xdr:colOff>1186920</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>42120</xdr:rowOff>
+      <xdr:rowOff>41040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1609,8 +1927,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3300480" y="7160760"/>
-          <a:ext cx="6929640" cy="1850400"/>
+          <a:off x="3303720" y="7160760"/>
+          <a:ext cx="6931800" cy="1849680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1632,7 +1950,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -1853,9 +2171,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1188000</xdr:colOff>
+      <xdr:colOff>1186920</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>63720</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1864,8 +2182,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3300480" y="7020000"/>
-          <a:ext cx="6929640" cy="1850400"/>
+          <a:off x="3303720" y="7020000"/>
+          <a:ext cx="6931800" cy="1849320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1887,7 +2205,517 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1300" spc="-1" strike="noStrike" u="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:uFillTx/>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>Instructions:</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>1. Add the names of all team members to the green box in row 1</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>2. Default values for all parameters go in line 6</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>3. Sample-specific parameters are entered in rows 7+</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>4. Default values from line 6 will be used for all cells left blank in rows 7+</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>5. Specify motor names and positions in columns R,S,T,U,V,W; leave blank for no motion</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>6. Specify detector position in column Q, blank means to </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="0" i="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>not move</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t> the detector </a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>6. Do not add rows above row 7</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>7. Do not add columns before column AI</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>711720</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>1440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1186920</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>62640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3303720" y="7020000"/>
+          <a:ext cx="6931800" cy="1849320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="73080">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="1" lang="en-US" sz="1300" spc="-1" strike="noStrike" u="sng">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:uFillTx/>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>Instructions:</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1300" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>1. Add the names of all team members to the green box in row 1</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>2. Default values for all parameters go in line 6</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>3. Sample-specific parameters are entered in rows 7+</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>4. Default values from line 6 will be used for all cells left blank in rows 7+</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>5. Specify motor names and positions in columns R,S,T,U,V,W; leave blank for no motion</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>6. Specify detector position in column Q, blank means to </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="0" i="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>not move</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t> the detector </a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>6. Do not add rows above row 7</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Bitstream Vera Sans"/>
+            </a:rPr>
+            <a:t>7. Do not add columns before column AI</a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>711720</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>1440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1186920</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>62640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3303720" y="7020000"/>
+          <a:ext cx="6931800" cy="1849320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="ffffff"/>
+        </a:solidFill>
+        <a:ln w="73080">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -2109,10 +2937,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
@@ -2175,7 +3003,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 13</v>
+        <v>Version: 14</v>
       </c>
       <c r="C2" s="6"/>
       <c r="H2" s="7" t="s">
@@ -3152,9 +3980,8 @@
       <c r="AF30" s="60"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="11">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:AE1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="C4:D4"/>
@@ -3167,70 +3994,70 @@
     <mergeCell ref="AF4:AH4"/>
   </mergeCells>
   <dataValidations count="15">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Z6:AE30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Z6:AE30" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I30" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E30" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AF6:AH6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AF6:AH6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G7:G30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G7:G30" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6 T6 R7:W30" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6 T6 R7:W30" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q6 S6 U6:Y6" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q6 S6 U6:Y6" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 C6:C30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 C6:C30" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3252,10 +4079,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
@@ -3318,7 +4145,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 13</v>
+        <v>Version: 14</v>
       </c>
       <c r="C2" s="6"/>
       <c r="E2" s="7" t="s">
@@ -4325,9 +5152,8 @@
       <c r="AF30" s="60"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="12">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:AE1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="H2:I2"/>
@@ -4341,70 +5167,70 @@
     <mergeCell ref="AF4:AH4"/>
   </mergeCells>
   <dataValidations count="15">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Z6:AE30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Z6:AE30" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I30" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E30" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AF6:AH6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AF6:AH6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G7:G30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G7:G30" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6 T6 R7:W30 Y7:Y30" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6 T6 R7:W30 Y7:Y30" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q6 S6 U6:Y6" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q6 S6 U6:Y6" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C30" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4426,10 +5252,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
@@ -4492,7 +5318,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 13</v>
+        <v>Version: 14</v>
       </c>
       <c r="C2" s="6"/>
       <c r="H2" s="7" t="s">
@@ -5491,9 +6317,8 @@
       <c r="AF30" s="60"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="11">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="E1:AE1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="C4:D4"/>
@@ -5506,74 +6331,74 @@
     <mergeCell ref="AF4:AH4"/>
   </mergeCells>
   <dataValidations count="16">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Z6:AE30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Z6:AE30" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I30" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E30" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
       <formula1>1</formula1>
       <formula2>24</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AF6:AH6" type="decimal">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AF6:AH6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G7:G30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G7:G30" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R30 T6 V7:W30" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R30 T6 V7:W30" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q6 S6 U6:Y6" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q6 S6 U6:Y6" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 C6:C30" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 C6:C30" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S7:U30 Y7:Y30" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S7:U30 Y7:Y30" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5588,13 +6413,2349 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="B1:AH30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="29.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="22.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="26" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="32" min="32" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="33" min="33" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="34" min="34" style="0" width="24.87"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="6" t="str">
+        <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
+        <v>Version: 14</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="H2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
+      <c r="AE2" s="10"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="0"/>
+      <c r="AB3" s="0"/>
+      <c r="AC3" s="0"/>
+      <c r="AD3" s="0"/>
+      <c r="AE3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2"/>
+      <c r="C4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="16"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="17"/>
+    </row>
+    <row r="5" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="18"/>
+      <c r="C5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="T5" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="U5" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="V5" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="W5" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="X5" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y5" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB5" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC5" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD5" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE5" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF5" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG5" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH5" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" s="29" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="30"/>
+      <c r="C6" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="O6" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="P6" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="S6" s="45"/>
+      <c r="T6" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="U6" s="45"/>
+      <c r="V6" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="W6" s="45"/>
+      <c r="X6" s="45"/>
+      <c r="Y6" s="45"/>
+      <c r="Z6" s="46" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AA6" s="47" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AB6" s="47" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="47" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AD6" s="47" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AE6" s="48" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="49"/>
+      <c r="AG6" s="42"/>
+      <c r="AH6" s="42"/>
+    </row>
+    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="50"/>
+      <c r="C7" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="52"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="56"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="Y7" s="62"/>
+      <c r="Z7" s="57"/>
+      <c r="AA7" s="58"/>
+      <c r="AB7" s="58"/>
+      <c r="AC7" s="58"/>
+      <c r="AD7" s="58"/>
+      <c r="AE7" s="59"/>
+      <c r="AF7" s="60"/>
+    </row>
+    <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="50"/>
+      <c r="C8" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="52"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="56"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="56"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="Y8" s="62"/>
+      <c r="Z8" s="57"/>
+      <c r="AA8" s="58"/>
+      <c r="AB8" s="58"/>
+      <c r="AC8" s="58"/>
+      <c r="AD8" s="58"/>
+      <c r="AE8" s="59"/>
+      <c r="AF8" s="60"/>
+    </row>
+    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="50"/>
+      <c r="C9" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="56"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="Y9" s="62"/>
+      <c r="Z9" s="57"/>
+      <c r="AA9" s="58"/>
+      <c r="AB9" s="58"/>
+      <c r="AC9" s="58"/>
+      <c r="AD9" s="58"/>
+      <c r="AE9" s="59"/>
+      <c r="AF9" s="60"/>
+    </row>
+    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="50"/>
+      <c r="C10" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="56"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="Y10" s="62"/>
+      <c r="Z10" s="57"/>
+      <c r="AA10" s="58"/>
+      <c r="AB10" s="58"/>
+      <c r="AC10" s="58"/>
+      <c r="AD10" s="58"/>
+      <c r="AE10" s="59"/>
+      <c r="AF10" s="60"/>
+    </row>
+    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="50"/>
+      <c r="C11" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="56"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="Y11" s="62"/>
+      <c r="Z11" s="57"/>
+      <c r="AA11" s="58"/>
+      <c r="AB11" s="58"/>
+      <c r="AC11" s="58"/>
+      <c r="AD11" s="58"/>
+      <c r="AE11" s="59"/>
+      <c r="AF11" s="60"/>
+    </row>
+    <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="50"/>
+      <c r="C12" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="56"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="Y12" s="62"/>
+      <c r="Z12" s="57"/>
+      <c r="AA12" s="58"/>
+      <c r="AB12" s="58"/>
+      <c r="AC12" s="58"/>
+      <c r="AD12" s="58"/>
+      <c r="AE12" s="59"/>
+      <c r="AF12" s="60"/>
+    </row>
+    <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="50"/>
+      <c r="C13" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="56"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="Y13" s="62"/>
+      <c r="Z13" s="57"/>
+      <c r="AA13" s="58"/>
+      <c r="AB13" s="58"/>
+      <c r="AC13" s="58"/>
+      <c r="AD13" s="58"/>
+      <c r="AE13" s="59"/>
+      <c r="AF13" s="60"/>
+    </row>
+    <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="50"/>
+      <c r="C14" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="55"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="55"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="56"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="Y14" s="62"/>
+      <c r="Z14" s="57"/>
+      <c r="AA14" s="58"/>
+      <c r="AB14" s="58"/>
+      <c r="AC14" s="58"/>
+      <c r="AD14" s="58"/>
+      <c r="AE14" s="59"/>
+      <c r="AF14" s="60"/>
+    </row>
+    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="50"/>
+      <c r="C15" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="56"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="Y15" s="62"/>
+      <c r="Z15" s="57"/>
+      <c r="AA15" s="58"/>
+      <c r="AB15" s="58"/>
+      <c r="AC15" s="58"/>
+      <c r="AD15" s="58"/>
+      <c r="AE15" s="59"/>
+      <c r="AF15" s="60"/>
+    </row>
+    <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="50"/>
+      <c r="C16" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="55"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="56"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="Y16" s="62"/>
+      <c r="Z16" s="57"/>
+      <c r="AA16" s="58"/>
+      <c r="AB16" s="58"/>
+      <c r="AC16" s="58"/>
+      <c r="AD16" s="58"/>
+      <c r="AE16" s="59"/>
+      <c r="AF16" s="60"/>
+    </row>
+    <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B17" s="50"/>
+      <c r="C17" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="55"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="55"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="56"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="Y17" s="62"/>
+      <c r="Z17" s="57"/>
+      <c r="AA17" s="58"/>
+      <c r="AB17" s="58"/>
+      <c r="AC17" s="58"/>
+      <c r="AD17" s="58"/>
+      <c r="AE17" s="59"/>
+      <c r="AF17" s="60"/>
+    </row>
+    <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="50"/>
+      <c r="C18" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="56"/>
+      <c r="N18" s="55"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="56"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="Y18" s="62"/>
+      <c r="Z18" s="57"/>
+      <c r="AA18" s="58"/>
+      <c r="AB18" s="58"/>
+      <c r="AC18" s="58"/>
+      <c r="AD18" s="58"/>
+      <c r="AE18" s="59"/>
+      <c r="AF18" s="60"/>
+    </row>
+    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="50"/>
+      <c r="C19" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="55"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="56"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="Y19" s="62"/>
+      <c r="Z19" s="57"/>
+      <c r="AA19" s="58"/>
+      <c r="AB19" s="58"/>
+      <c r="AC19" s="58"/>
+      <c r="AD19" s="58"/>
+      <c r="AE19" s="59"/>
+      <c r="AF19" s="60"/>
+    </row>
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="50"/>
+      <c r="C20" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="29"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="55"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="55"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="56"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="Y20" s="62"/>
+      <c r="Z20" s="57"/>
+      <c r="AA20" s="58"/>
+      <c r="AB20" s="58"/>
+      <c r="AC20" s="58"/>
+      <c r="AD20" s="58"/>
+      <c r="AE20" s="59"/>
+      <c r="AF20" s="60"/>
+    </row>
+    <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B21" s="50"/>
+      <c r="C21" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="56"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="Y21" s="62"/>
+      <c r="Z21" s="57"/>
+      <c r="AA21" s="58"/>
+      <c r="AB21" s="58"/>
+      <c r="AC21" s="58"/>
+      <c r="AD21" s="58"/>
+      <c r="AE21" s="59"/>
+      <c r="AF21" s="60"/>
+    </row>
+    <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B22" s="50"/>
+      <c r="C22" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="56"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="Y22" s="62"/>
+      <c r="Z22" s="57"/>
+      <c r="AA22" s="58"/>
+      <c r="AB22" s="58"/>
+      <c r="AC22" s="58"/>
+      <c r="AD22" s="58"/>
+      <c r="AE22" s="59"/>
+      <c r="AF22" s="60"/>
+    </row>
+    <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="50"/>
+      <c r="C23" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="56"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="Y23" s="62"/>
+      <c r="Z23" s="57"/>
+      <c r="AA23" s="58"/>
+      <c r="AB23" s="58"/>
+      <c r="AC23" s="58"/>
+      <c r="AD23" s="58"/>
+      <c r="AE23" s="59"/>
+      <c r="AF23" s="60"/>
+    </row>
+    <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="50"/>
+      <c r="C24" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="29"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="56"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="Y24" s="62"/>
+      <c r="Z24" s="57"/>
+      <c r="AA24" s="58"/>
+      <c r="AB24" s="58"/>
+      <c r="AC24" s="58"/>
+      <c r="AD24" s="58"/>
+      <c r="AE24" s="59"/>
+      <c r="AF24" s="60"/>
+    </row>
+    <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="50"/>
+      <c r="C25" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="56"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="Y25" s="62"/>
+      <c r="Z25" s="57"/>
+      <c r="AA25" s="58"/>
+      <c r="AB25" s="58"/>
+      <c r="AC25" s="58"/>
+      <c r="AD25" s="58"/>
+      <c r="AE25" s="59"/>
+      <c r="AF25" s="60"/>
+    </row>
+    <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B26" s="50"/>
+      <c r="C26" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="55"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="56"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="Y26" s="62"/>
+      <c r="Z26" s="57"/>
+      <c r="AA26" s="58"/>
+      <c r="AB26" s="58"/>
+      <c r="AC26" s="58"/>
+      <c r="AD26" s="58"/>
+      <c r="AE26" s="59"/>
+      <c r="AF26" s="60"/>
+    </row>
+    <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="50"/>
+      <c r="C27" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="29"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="55"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="55"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="56"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="Y27" s="62"/>
+      <c r="Z27" s="57"/>
+      <c r="AA27" s="58"/>
+      <c r="AB27" s="58"/>
+      <c r="AC27" s="58"/>
+      <c r="AD27" s="58"/>
+      <c r="AE27" s="59"/>
+      <c r="AF27" s="60"/>
+    </row>
+    <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B28" s="50"/>
+      <c r="C28" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="29"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="55"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="56"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="Y28" s="62"/>
+      <c r="Z28" s="57"/>
+      <c r="AA28" s="58"/>
+      <c r="AB28" s="58"/>
+      <c r="AC28" s="58"/>
+      <c r="AD28" s="58"/>
+      <c r="AE28" s="59"/>
+      <c r="AF28" s="60"/>
+    </row>
+    <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="50"/>
+      <c r="C29" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="29"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="55"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="55"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="56"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="Y29" s="62"/>
+      <c r="Z29" s="57"/>
+      <c r="AA29" s="58"/>
+      <c r="AB29" s="58"/>
+      <c r="AC29" s="58"/>
+      <c r="AD29" s="58"/>
+      <c r="AE29" s="59"/>
+      <c r="AF29" s="60"/>
+    </row>
+    <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="50"/>
+      <c r="C30" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="29"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="55"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="55"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="56"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="Y30" s="62"/>
+      <c r="Z30" s="57"/>
+      <c r="AA30" s="58"/>
+      <c r="AB30" s="58"/>
+      <c r="AC30" s="58"/>
+      <c r="AD30" s="58"/>
+      <c r="AE30" s="59"/>
+      <c r="AF30" s="60"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:Y4"/>
+    <mergeCell ref="Z4:AE4"/>
+    <mergeCell ref="AF4:AH4"/>
+  </mergeCells>
+  <dataValidations count="16">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Z6:AE30" type="list">
+      <formula1>"True,False"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I30" type="list">
+      <formula1>"K,L3,L2,L1"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
+      <formula1>"unfocused,focused"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E30" type="whole">
+      <formula1>0</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
+      <formula1>1</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AF6:AH6" type="decimal">
+      <formula1>-0.1</formula1>
+      <formula2>8</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6" type="list">
+      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G7:G30" type="list">
+      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+      <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R30 T6 V7:W30" type="none">
+      <formula1>-150</formula1>
+      <formula2>150</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
+      <formula1>1</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q6 S6 U6:Y6" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 C6:C30" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S7:U30 Y7:Y30" type="none">
+      <formula1>-150</formula1>
+      <formula2>150</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:AH30"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="6" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="bottomRight" activeCell="K6" activeCellId="0" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="29.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="22.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="22" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="26" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="32" min="32" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="33" min="33" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="34" min="34" style="0" width="24.87"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="6" t="str">
+        <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
+        <v>Version: 14</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="H2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
+      <c r="AE2" s="10"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="0"/>
+      <c r="AB3" s="0"/>
+      <c r="AC3" s="0"/>
+      <c r="AD3" s="0"/>
+      <c r="AE3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2"/>
+      <c r="C4" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="16"/>
+      <c r="AC4" s="16"/>
+      <c r="AD4" s="16"/>
+      <c r="AE4" s="16"/>
+      <c r="AF4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="17"/>
+    </row>
+    <row r="5" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="18"/>
+      <c r="C5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="T5" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="U5" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="V5" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="W5" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="X5" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y5" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="AA5" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB5" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC5" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD5" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE5" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF5" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG5" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH5" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" s="29" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="30"/>
+      <c r="C6" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="O6" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="P6" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="S6" s="45"/>
+      <c r="T6" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="U6" s="45"/>
+      <c r="V6" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="W6" s="45"/>
+      <c r="X6" s="45"/>
+      <c r="Y6" s="45"/>
+      <c r="Z6" s="46" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AA6" s="47" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AB6" s="47" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="47" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AD6" s="47" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="AE6" s="48" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="AF6" s="49"/>
+      <c r="AG6" s="42"/>
+      <c r="AH6" s="42"/>
+    </row>
+    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B7" s="50"/>
+      <c r="C7" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="52"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="56"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="Y7" s="62"/>
+      <c r="Z7" s="57"/>
+      <c r="AA7" s="58"/>
+      <c r="AB7" s="58"/>
+      <c r="AC7" s="58"/>
+      <c r="AD7" s="58"/>
+      <c r="AE7" s="59"/>
+      <c r="AF7" s="60"/>
+    </row>
+    <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="50"/>
+      <c r="C8" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="52"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="56"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="56"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
+      <c r="Y8" s="62"/>
+      <c r="Z8" s="57"/>
+      <c r="AA8" s="58"/>
+      <c r="AB8" s="58"/>
+      <c r="AC8" s="58"/>
+      <c r="AD8" s="58"/>
+      <c r="AE8" s="59"/>
+      <c r="AF8" s="60"/>
+    </row>
+    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="50"/>
+      <c r="C9" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="55"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="55"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="56"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
+      <c r="Y9" s="62"/>
+      <c r="Z9" s="57"/>
+      <c r="AA9" s="58"/>
+      <c r="AB9" s="58"/>
+      <c r="AC9" s="58"/>
+      <c r="AD9" s="58"/>
+      <c r="AE9" s="59"/>
+      <c r="AF9" s="60"/>
+    </row>
+    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B10" s="50"/>
+      <c r="C10" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="55"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="55"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="56"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="Y10" s="62"/>
+      <c r="Z10" s="57"/>
+      <c r="AA10" s="58"/>
+      <c r="AB10" s="58"/>
+      <c r="AC10" s="58"/>
+      <c r="AD10" s="58"/>
+      <c r="AE10" s="59"/>
+      <c r="AF10" s="60"/>
+    </row>
+    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B11" s="50"/>
+      <c r="C11" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="56"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
+      <c r="Y11" s="62"/>
+      <c r="Z11" s="57"/>
+      <c r="AA11" s="58"/>
+      <c r="AB11" s="58"/>
+      <c r="AC11" s="58"/>
+      <c r="AD11" s="58"/>
+      <c r="AE11" s="59"/>
+      <c r="AF11" s="60"/>
+    </row>
+    <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="50"/>
+      <c r="C12" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="56"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
+      <c r="Y12" s="62"/>
+      <c r="Z12" s="57"/>
+      <c r="AA12" s="58"/>
+      <c r="AB12" s="58"/>
+      <c r="AC12" s="58"/>
+      <c r="AD12" s="58"/>
+      <c r="AE12" s="59"/>
+      <c r="AF12" s="60"/>
+    </row>
+    <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B13" s="50"/>
+      <c r="C13" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="55"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="56"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
+      <c r="Y13" s="62"/>
+      <c r="Z13" s="57"/>
+      <c r="AA13" s="58"/>
+      <c r="AB13" s="58"/>
+      <c r="AC13" s="58"/>
+      <c r="AD13" s="58"/>
+      <c r="AE13" s="59"/>
+      <c r="AF13" s="60"/>
+    </row>
+    <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="50"/>
+      <c r="C14" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="55"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="55"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="56"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="Y14" s="62"/>
+      <c r="Z14" s="57"/>
+      <c r="AA14" s="58"/>
+      <c r="AB14" s="58"/>
+      <c r="AC14" s="58"/>
+      <c r="AD14" s="58"/>
+      <c r="AE14" s="59"/>
+      <c r="AF14" s="60"/>
+    </row>
+    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="50"/>
+      <c r="C15" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="56"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="Y15" s="62"/>
+      <c r="Z15" s="57"/>
+      <c r="AA15" s="58"/>
+      <c r="AB15" s="58"/>
+      <c r="AC15" s="58"/>
+      <c r="AD15" s="58"/>
+      <c r="AE15" s="59"/>
+      <c r="AF15" s="60"/>
+    </row>
+    <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="50"/>
+      <c r="C16" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="55"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="55"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="56"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+      <c r="Y16" s="62"/>
+      <c r="Z16" s="57"/>
+      <c r="AA16" s="58"/>
+      <c r="AB16" s="58"/>
+      <c r="AC16" s="58"/>
+      <c r="AD16" s="58"/>
+      <c r="AE16" s="59"/>
+      <c r="AF16" s="60"/>
+    </row>
+    <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B17" s="50"/>
+      <c r="C17" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="55"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="55"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="56"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="Y17" s="62"/>
+      <c r="Z17" s="57"/>
+      <c r="AA17" s="58"/>
+      <c r="AB17" s="58"/>
+      <c r="AC17" s="58"/>
+      <c r="AD17" s="58"/>
+      <c r="AE17" s="59"/>
+      <c r="AF17" s="60"/>
+    </row>
+    <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="50"/>
+      <c r="C18" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="56"/>
+      <c r="N18" s="55"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="56"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="Y18" s="62"/>
+      <c r="Z18" s="57"/>
+      <c r="AA18" s="58"/>
+      <c r="AB18" s="58"/>
+      <c r="AC18" s="58"/>
+      <c r="AD18" s="58"/>
+      <c r="AE18" s="59"/>
+      <c r="AF18" s="60"/>
+    </row>
+    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="50"/>
+      <c r="C19" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="55"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="56"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="Y19" s="62"/>
+      <c r="Z19" s="57"/>
+      <c r="AA19" s="58"/>
+      <c r="AB19" s="58"/>
+      <c r="AC19" s="58"/>
+      <c r="AD19" s="58"/>
+      <c r="AE19" s="59"/>
+      <c r="AF19" s="60"/>
+    </row>
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="50"/>
+      <c r="C20" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="29"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="55"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="55"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="56"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="Y20" s="62"/>
+      <c r="Z20" s="57"/>
+      <c r="AA20" s="58"/>
+      <c r="AB20" s="58"/>
+      <c r="AC20" s="58"/>
+      <c r="AD20" s="58"/>
+      <c r="AE20" s="59"/>
+      <c r="AF20" s="60"/>
+    </row>
+    <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B21" s="50"/>
+      <c r="C21" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="56"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="Y21" s="62"/>
+      <c r="Z21" s="57"/>
+      <c r="AA21" s="58"/>
+      <c r="AB21" s="58"/>
+      <c r="AC21" s="58"/>
+      <c r="AD21" s="58"/>
+      <c r="AE21" s="59"/>
+      <c r="AF21" s="60"/>
+    </row>
+    <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B22" s="50"/>
+      <c r="C22" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="56"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="Y22" s="62"/>
+      <c r="Z22" s="57"/>
+      <c r="AA22" s="58"/>
+      <c r="AB22" s="58"/>
+      <c r="AC22" s="58"/>
+      <c r="AD22" s="58"/>
+      <c r="AE22" s="59"/>
+      <c r="AF22" s="60"/>
+    </row>
+    <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="50"/>
+      <c r="C23" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="56"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="Y23" s="62"/>
+      <c r="Z23" s="57"/>
+      <c r="AA23" s="58"/>
+      <c r="AB23" s="58"/>
+      <c r="AC23" s="58"/>
+      <c r="AD23" s="58"/>
+      <c r="AE23" s="59"/>
+      <c r="AF23" s="60"/>
+    </row>
+    <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="50"/>
+      <c r="C24" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="29"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="56"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="Y24" s="62"/>
+      <c r="Z24" s="57"/>
+      <c r="AA24" s="58"/>
+      <c r="AB24" s="58"/>
+      <c r="AC24" s="58"/>
+      <c r="AD24" s="58"/>
+      <c r="AE24" s="59"/>
+      <c r="AF24" s="60"/>
+    </row>
+    <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="50"/>
+      <c r="C25" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="56"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="Y25" s="62"/>
+      <c r="Z25" s="57"/>
+      <c r="AA25" s="58"/>
+      <c r="AB25" s="58"/>
+      <c r="AC25" s="58"/>
+      <c r="AD25" s="58"/>
+      <c r="AE25" s="59"/>
+      <c r="AF25" s="60"/>
+    </row>
+    <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B26" s="50"/>
+      <c r="C26" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="55"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="56"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="Y26" s="62"/>
+      <c r="Z26" s="57"/>
+      <c r="AA26" s="58"/>
+      <c r="AB26" s="58"/>
+      <c r="AC26" s="58"/>
+      <c r="AD26" s="58"/>
+      <c r="AE26" s="59"/>
+      <c r="AF26" s="60"/>
+    </row>
+    <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="50"/>
+      <c r="C27" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="29"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="55"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="55"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="56"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="Y27" s="62"/>
+      <c r="Z27" s="57"/>
+      <c r="AA27" s="58"/>
+      <c r="AB27" s="58"/>
+      <c r="AC27" s="58"/>
+      <c r="AD27" s="58"/>
+      <c r="AE27" s="59"/>
+      <c r="AF27" s="60"/>
+    </row>
+    <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B28" s="50"/>
+      <c r="C28" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="29"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="55"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="56"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="Y28" s="62"/>
+      <c r="Z28" s="57"/>
+      <c r="AA28" s="58"/>
+      <c r="AB28" s="58"/>
+      <c r="AC28" s="58"/>
+      <c r="AD28" s="58"/>
+      <c r="AE28" s="59"/>
+      <c r="AF28" s="60"/>
+    </row>
+    <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="50"/>
+      <c r="C29" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="29"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="55"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="55"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="56"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="Y29" s="62"/>
+      <c r="Z29" s="57"/>
+      <c r="AA29" s="58"/>
+      <c r="AB29" s="58"/>
+      <c r="AC29" s="58"/>
+      <c r="AD29" s="58"/>
+      <c r="AE29" s="59"/>
+      <c r="AF29" s="60"/>
+    </row>
+    <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="50"/>
+      <c r="C30" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="29"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="55"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="55"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="56"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="Y30" s="62"/>
+      <c r="Z30" s="57"/>
+      <c r="AA30" s="58"/>
+      <c r="AB30" s="58"/>
+      <c r="AC30" s="58"/>
+      <c r="AD30" s="58"/>
+      <c r="AE30" s="59"/>
+      <c r="AF30" s="60"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="Q4:Y4"/>
+    <mergeCell ref="Z4:AE4"/>
+    <mergeCell ref="AF4:AH4"/>
+  </mergeCells>
+  <dataValidations count="16">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Z6:AE30" type="list">
+      <formula1>"True,False"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I30" type="list">
+      <formula1>"K,L3,L2,L1"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J30" type="list">
+      <formula1>"unfocused,focused"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E6:E30" type="whole">
+      <formula1>0</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:B30" type="whole">
+      <formula1>1</formula1>
+      <formula2>24</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AF6:AH6" type="decimal">
+      <formula1>-0.1</formula1>
+      <formula2>8</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6" type="list">
+      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G7:G30" type="list">
+      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+      <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H30" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:R30 T6 V7:W30" type="none">
+      <formula1>-150</formula1>
+      <formula2>150</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
+      <formula1>1</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="Q6 S6 U6:Y6" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 C6:C30" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S7:U30 Y7:Y30" type="none">
+      <formula1>-150</formula1>
+      <formula2>150</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -5613,7 +8774,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="64"/>
     </row>
@@ -5733,10 +8894,18 @@
         <v>77</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
added resonant reflectivity automation
+ move dcm_roll value to BMM_configuration.ini
+ add backoff into post_document()
+ explicitly enable ROISTAT plugin for Pilatus
</commit_message>
<xml_diff>
--- a/startup/xlsx/grid.xlsx
+++ b/startup/xlsx/grid.xlsx
@@ -690,7 +690,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="81">
   <si>
     <t xml:space="preserve">Grid</t>
   </si>
@@ -930,6 +930,9 @@
   </si>
   <si>
     <t xml:space="preserve">update validity for plotting mode columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">added resonant reflectivity spreadsheet</t>
   </si>
 </sst>
 </file>
@@ -1668,9 +1671,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1081440</xdr:colOff>
+      <xdr:colOff>1081080</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>55440</xdr:rowOff>
+      <xdr:rowOff>55080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1679,8 +1682,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3199680" y="7013160"/>
-          <a:ext cx="6932880" cy="1848960"/>
+          <a:off x="3200400" y="7013160"/>
+          <a:ext cx="6933240" cy="1848600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1923,9 +1926,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1186560</xdr:colOff>
+      <xdr:colOff>1186200</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>40680</xdr:rowOff>
+      <xdr:rowOff>40320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1934,8 +1937,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3304800" y="7160760"/>
-          <a:ext cx="6932880" cy="1848960"/>
+          <a:off x="3305520" y="7160760"/>
+          <a:ext cx="6933240" cy="1848600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2178,9 +2181,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1186560</xdr:colOff>
+      <xdr:colOff>1186200</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2189,8 +2192,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3304800" y="7020000"/>
-          <a:ext cx="6932880" cy="1848960"/>
+          <a:off x="3305520" y="7020000"/>
+          <a:ext cx="6933240" cy="1848600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2433,9 +2436,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1186560</xdr:colOff>
+      <xdr:colOff>1186200</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2444,8 +2447,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3304800" y="7020000"/>
-          <a:ext cx="6932880" cy="1848960"/>
+          <a:off x="3305520" y="7020000"/>
+          <a:ext cx="6933240" cy="1848600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2688,9 +2691,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1186560</xdr:colOff>
+      <xdr:colOff>1186200</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
+      <xdr:rowOff>61920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2699,8 +2702,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3304800" y="7020000"/>
-          <a:ext cx="6932880" cy="1848960"/>
+          <a:off x="3305520" y="7020000"/>
+          <a:ext cx="6933240" cy="1848600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2944,10 +2947,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G6" activeCellId="0" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
@@ -3010,7 +3013,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 15</v>
+        <v>Version: 16</v>
       </c>
       <c r="C2" s="6"/>
       <c r="H2" s="7" t="s">
@@ -4085,7 +4088,7 @@
       <selection pane="bottomRight" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
@@ -4148,7 +4151,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 15</v>
+        <v>Version: 16</v>
       </c>
       <c r="C2" s="6"/>
       <c r="E2" s="7" t="s">
@@ -5218,12 +5221,12 @@
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G30" type="list">
+      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 C6:C30" type="list">
       <formula1>"Yes,No"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G30" type="list">
-      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -5254,7 +5257,7 @@
       <selection pane="bottomRight" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
@@ -5317,7 +5320,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 15</v>
+        <v>Version: 16</v>
       </c>
       <c r="C2" s="6"/>
       <c r="H2" s="7" t="s">
@@ -6382,13 +6385,13 @@
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G30" type="list">
+      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S7:U30 Y7:Y30" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G30" type="list">
-      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
-      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6418,7 +6421,7 @@
       <selection pane="bottomRight" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
@@ -6481,7 +6484,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 15</v>
+        <v>Version: 16</v>
       </c>
       <c r="C2" s="6"/>
       <c r="H2" s="7" t="s">
@@ -7546,13 +7549,13 @@
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G30" type="list">
+      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S7:U30 Y7:Y30" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G30" type="list">
-      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
-      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7582,7 +7585,7 @@
       <selection pane="bottomRight" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.01"/>
@@ -7645,7 +7648,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 15</v>
+        <v>Version: 16</v>
       </c>
       <c r="C2" s="6"/>
       <c r="H2" s="7" t="s">
@@ -8710,13 +8713,13 @@
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G30" type="list">
+      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S7:U30 Y7:Y30" type="none">
       <formula1>-150</formula1>
       <formula2>150</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G30" type="list">
-      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
-      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -8736,13 +8739,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
@@ -8761,7 +8764,8 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="n">
-        <v>15</v>
+        <f aca="false">MAX(A6:A41)</f>
+        <v>16</v>
       </c>
       <c r="B3" s="65"/>
     </row>
@@ -8895,6 +8899,14 @@
       </c>
       <c r="B20" s="0" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>